<commit_message>
Tested different diet types.
</commit_message>
<xml_diff>
--- a/Output/Test/Diets.xlsx
+++ b/Output/Test/Diets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sophi\Antarctic-Food-Optimisation\Output\Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F180E68-874B-4D35-B861-EFB5FEFD4ABF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9948E7AB-C589-40E4-AE20-0CBD9A1FAEF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F25FA96D-726B-4069-8BBB-7E5C86B0ABB0}"/>
   </bookViews>
@@ -35,15 +35,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="27">
   <si>
     <t>Excess calories (food waste)</t>
   </si>
   <si>
     <t>Batch 1</t>
-  </si>
-  <si>
-    <t>Full range, no objective</t>
   </si>
   <si>
     <t>Full range of food</t>
@@ -65,9 +62,6 @@
   </si>
   <si>
     <t>Cost / £</t>
-  </si>
-  <si>
-    <t>Emissions / CO2e</t>
   </si>
   <si>
     <t>Packaging waste / kg</t>
@@ -109,13 +103,19 @@
     <t>Cost / £ per person per day</t>
   </si>
   <si>
-    <t>Emissions / CO2e per person per day</t>
-  </si>
-  <si>
     <t>Excess calories (food waste) per person per day</t>
   </si>
   <si>
     <t>Packaging waste / g per person per day</t>
+  </si>
+  <si>
+    <t>Animal-based, no objective</t>
+  </si>
+  <si>
+    <t>Emissions / kg CO2e per person per day</t>
+  </si>
+  <si>
+    <t>Emissions / kg CO2e</t>
   </si>
 </sst>
 </file>
@@ -198,13 +198,27 @@
           <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
-            <a:pPr>
+            <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
               <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
+                  <a:sysClr val="windowText" lastClr="000000">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  </a:sysClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -212,12 +226,10 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-GB"/>
-              <a:t>Objective</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-GB" baseline="0"/>
-              <a:t> performance with different diets</a:t>
+              <a:rPr lang="en-GB" sz="1800" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Objective performance with different diets</a:t>
             </a:r>
             <a:endParaRPr lang="en-GB"/>
           </a:p>
@@ -235,13 +247,27 @@
         <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
         <a:lstStyle/>
         <a:p>
-          <a:pPr>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
             <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
+                <a:sysClr val="windowText" lastClr="000000">
                   <a:lumMod val="65000"/>
                   <a:lumOff val="35000"/>
-                </a:schemeClr>
+                </a:sysClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -255,15 +281,16 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$15</c:f>
+              <c:f>Sheet1!$A$20</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -273,34 +300,22 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
               <a:noFill/>
-              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$9:$G$9</c:f>
+              <c:f>Sheet1!$B$14:$G$14</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>Full range, no objective</c:v>
+                  <c:v>Animal-based, no objective</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Full range of food</c:v>
@@ -319,15 +334,15 @@
                 </c:pt>
               </c:strCache>
             </c:strRef>
-          </c:xVal>
-          <c:yVal>
+          </c:cat>
+          <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$15:$G$15</c:f>
+              <c:f>Sheet1!$B$20:$G$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>9.8231012658227854</c:v>
+                  <c:v>9.6939873417721518</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>9.6525316455696206</c:v>
@@ -346,11 +361,10 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
+          </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-57C0-4AF6-B8D9-23C1F415F74A}"/>
+              <c16:uniqueId val="{00000000-EA3C-448C-897E-0352A0F7850B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -359,44 +373,32 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$16</c:f>
+              <c:f>Sheet1!$A$21</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Emissions / CO2e per person per day</c:v>
+                  <c:v>Emissions / kg CO2e per person per day</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
               <a:noFill/>
-              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$9:$G$9</c:f>
+              <c:f>Sheet1!$B$14:$G$14</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>Full range, no objective</c:v>
+                  <c:v>Animal-based, no objective</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Full range of food</c:v>
@@ -415,15 +417,15 @@
                 </c:pt>
               </c:strCache>
             </c:strRef>
-          </c:xVal>
-          <c:yVal>
+          </c:cat>
+          <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$16:$G$16</c:f>
+              <c:f>Sheet1!$B$21:$G$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>8.8560126582278489</c:v>
+                  <c:v>12.047784810126583</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>8.7996835443037984</c:v>
@@ -432,213 +434,20 @@
                   <c:v>8.6708860759493671</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>8.8272151898734172</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>8.5718354430379744</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>8.8272151898734172</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>8.4971518987341774</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
+          </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-57C0-4AF6-B8D9-23C1F415F74A}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$A$17</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Packaging waste / g per person per day</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:strRef>
-              <c:f>Sheet1!$B$9:$G$9</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>Full range, no objective</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Full range of food</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Red meat mixed with 50% mycoprotein</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>No ruminent meat</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Vegetarian</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Vegan</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$B$17:$G$17</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>31.329113924050635</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>30.063291139240508</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>30.063291139240508</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>30.37974683544304</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>28.164556962025319</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>24.367088607594933</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-57C0-4AF6-B8D9-23C1F415F74A}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$A$18</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Excess calories (food waste) per person per day</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent4"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:strRef>
-              <c:f>Sheet1!$B$9:$G$9</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>Full range, no objective</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Full range of food</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Red meat mixed with 50% mycoprotein</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>No ruminent meat</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Vegetarian</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Vegan</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$B$18:$G$18</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>49.579113924050631</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>49.010759493670882</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>49.010759493670882</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>49.068354430379749</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>23.401582278481012</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5.6544303797468354</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-57C0-4AF6-B8D9-23C1F415F74A}"/>
+              <c16:uniqueId val="{00000001-EA3C-448C-897E-0352A0F7850B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -650,30 +459,19 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="551443792"/>
-        <c:axId val="551450448"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="551443792"/>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="288205600"/>
+        <c:axId val="288205184"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="288205600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -682,8 +480,8 @@
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -710,14 +508,19 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="551450448"/>
+        <c:crossAx val="288205184"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
       <c:valAx>
-        <c:axId val="551450448"/>
+        <c:axId val="288205184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="15"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -741,14 +544,8 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
+          <a:ln>
+            <a:noFill/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -772,9 +569,9 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="551443792"/>
+        <c:crossAx val="288205600"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -874,80 +671,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-              <a:lnSpc>
-                <a:spcPct val="100000"/>
-              </a:lnSpc>
-              <a:spcBef>
-                <a:spcPts val="0"/>
-              </a:spcBef>
-              <a:spcAft>
-                <a:spcPts val="0"/>
-              </a:spcAft>
-              <a:buClrTx/>
-              <a:buSzTx/>
-              <a:buFontTx/>
-              <a:buNone/>
-              <a:tabLst/>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:sysClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-GB" sz="1800" b="0" i="0" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
-              <a:t>Objective performance with different diets</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-GB">
-              <a:effectLst/>
-            </a:endParaRPr>
-          </a:p>
-          <a:p>
-            <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-              <a:lnSpc>
-                <a:spcPct val="100000"/>
-              </a:lnSpc>
-              <a:spcBef>
-                <a:spcPts val="0"/>
-              </a:spcBef>
-              <a:spcAft>
-                <a:spcPts val="0"/>
-              </a:spcAft>
-              <a:buClrTx/>
-              <a:buSzTx/>
-              <a:buFontTx/>
-              <a:buNone/>
-              <a:tabLst/>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:sysClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-GB"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -960,27 +683,13 @@
         <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buClrTx/>
-            <a:buSzTx/>
-            <a:buFontTx/>
-            <a:buNone/>
-            <a:tabLst/>
+          <a:pPr>
             <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000">
+                <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
                   <a:lumOff val="35000"/>
-                </a:sysClr>
+                </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -1003,7 +712,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$15</c:f>
+              <c:f>Sheet1!$A$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1024,22 +733,25 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$C$9:$G$9</c:f>
+              <c:f>Sheet1!$B$1:$G$1</c:f>
               <c:strCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>Animal-based, no objective</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>Full range of food</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>Red meat mixed with 50% mycoprotein</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>No ruminent meat</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>Vegetarian</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>Vegan</c:v>
                 </c:pt>
               </c:strCache>
@@ -1047,31 +759,34 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$15:$G$15</c:f>
+              <c:f>Sheet1!$B$7:$G$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>9.6525316455696206</c:v>
+                  <c:v>10.37619372442019</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.6408227848101262</c:v>
+                  <c:v>9.2919508867667115</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.6686708860759492</c:v>
+                  <c:v>9.3086630286493861</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10.609810126582278</c:v>
+                  <c:v>9.3935879945429743</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10.58481012658228</c:v>
+                  <c:v>10.898021828103683</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.254433833560709</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-0A2F-4253-9A15-9841A3175F53}"/>
+              <c16:uniqueId val="{00000000-6FDF-4F9F-A94E-15560ED04357}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1080,11 +795,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$16</c:f>
+              <c:f>Sheet1!$A$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Emissions / CO2e per person per day</c:v>
+                  <c:v>Emissions / kg CO2e per person per day</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1101,22 +816,25 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$C$9:$G$9</c:f>
+              <c:f>Sheet1!$B$1:$G$1</c:f>
               <c:strCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>Animal-based, no objective</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>Full range of food</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>Red meat mixed with 50% mycoprotein</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>No ruminent meat</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>Vegetarian</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>Vegan</c:v>
                 </c:pt>
               </c:strCache>
@@ -1124,31 +842,34 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$16:$G$16</c:f>
+              <c:f>Sheet1!$B$8:$G$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>8.7996835443037984</c:v>
+                  <c:v>12.251364256480219</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.6708860759493671</c:v>
+                  <c:v>8.4229195088676665</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.5718354430379744</c:v>
+                  <c:v>8.1459754433833567</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.8272151898734172</c:v>
+                  <c:v>7.8782401091405188</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.4971518987341774</c:v>
+                  <c:v>8.5354706684856758</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.2186221009549794</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-0A2F-4253-9A15-9841A3175F53}"/>
+              <c16:uniqueId val="{00000001-6FDF-4F9F-A94E-15560ED04357}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1157,7 +878,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$17</c:f>
+              <c:f>Sheet1!$A$9</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1178,22 +899,25 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$C$9:$G$9</c:f>
+              <c:f>Sheet1!$B$1:$G$1</c:f>
               <c:strCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>Animal-based, no objective</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>Full range of food</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>Red meat mixed with 50% mycoprotein</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>No ruminent meat</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>Vegetarian</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>Vegan</c:v>
                 </c:pt>
               </c:strCache>
@@ -1201,31 +925,34 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$17:$G$17</c:f>
+              <c:f>Sheet1!$B$9:$G$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>30.063291139240508</c:v>
+                  <c:v>42.291950886766713</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>30.063291139240508</c:v>
+                  <c:v>39.563437926330153</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30.37974683544304</c:v>
+                  <c:v>39.563437926330153</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>28.164556962025319</c:v>
+                  <c:v>39.563437926330153</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>24.367088607594933</c:v>
+                  <c:v>32.401091405184175</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>17.053206002728512</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-0A2F-4253-9A15-9841A3175F53}"/>
+              <c16:uniqueId val="{00000002-6FDF-4F9F-A94E-15560ED04357}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1234,7 +961,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$18</c:f>
+              <c:f>Sheet1!$A$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1255,22 +982,25 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$C$9:$G$9</c:f>
+              <c:f>Sheet1!$B$1:$G$1</c:f>
               <c:strCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>Animal-based, no objective</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>Full range of food</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>Red meat mixed with 50% mycoprotein</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>No ruminent meat</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>Vegetarian</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>Vegan</c:v>
                 </c:pt>
               </c:strCache>
@@ -1278,31 +1008,34 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$18:$G$18</c:f>
+              <c:f>Sheet1!$B$10:$G$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>49.010759493670882</c:v>
+                  <c:v>1282.4641882673943</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>49.010759493670882</c:v>
+                  <c:v>437.40620736698497</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>49.068354430379749</c:v>
+                  <c:v>437.40620736698497</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>23.401582278481012</c:v>
+                  <c:v>431.04809004092772</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.6544303797468354</c:v>
+                  <c:v>354.53035470668488</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.5665075034106408</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-0A2F-4253-9A15-9841A3175F53}"/>
+              <c16:uniqueId val="{00000003-6FDF-4F9F-A94E-15560ED04357}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1316,11 +1049,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="551502864"/>
-        <c:axId val="551494544"/>
+        <c:axId val="2060987872"/>
+        <c:axId val="2060989120"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="551502864"/>
+        <c:axId val="2060987872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1363,7 +1096,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="551494544"/>
+        <c:crossAx val="2060989120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1371,9 +1104,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="551494544"/>
+        <c:axId val="2060989120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="20"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1422,7 +1156,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="551502864"/>
+        <c:crossAx val="2060987872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1590,522 +1324,6 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2608,27 +1826,530 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>149469</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>55683</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>439492</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>71642</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>454269</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>175845</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>454147</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>56989</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="11" name="Chart 10">
+        <xdr:cNvPr id="9" name="Chart 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4A4DD830-0748-BD83-4D95-72055A2EF6FD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B8B2844-7F56-EDDE-F218-A1E5C977CEA4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2648,23 +2369,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>52754</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>8792</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>371395</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>70436</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>536331</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>105508</xdr:rowOff>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>352185</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>64033</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="14" name="Chart 13">
+        <xdr:cNvPr id="10" name="Chart 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B909CE7-3207-281D-A31D-3A0CBB24F3CC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F09E7B67-CC8C-B745-9EFB-3AC09EFE6879}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2982,10 +2703,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3CA0575-3F52-46AB-9BBD-3353A2249647}">
-  <dimension ref="A1:J38"/>
+  <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G22" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="U33" sqref="U33"/>
+    <sheetView tabSelected="1" topLeftCell="J15" zoomScale="119" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3003,30 +2724,30 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3">
-        <v>27148</v>
+        <v>30423</v>
       </c>
       <c r="C3">
         <v>27244</v>
@@ -3036,14 +2757,20 @@
       </c>
       <c r="E3">
         <v>27542</v>
+      </c>
+      <c r="F3">
+        <v>31953</v>
+      </c>
+      <c r="G3">
+        <v>27134</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="B4">
-        <v>24685</v>
+        <v>35921</v>
       </c>
       <c r="C4">
         <v>24696</v>
@@ -3053,14 +2780,20 @@
       </c>
       <c r="E4">
         <v>23099</v>
+      </c>
+      <c r="F4">
+        <v>25026</v>
+      </c>
+      <c r="G4">
+        <v>24097</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B5">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="C5">
         <v>116</v>
@@ -3070,6 +2803,12 @@
       </c>
       <c r="E5">
         <v>116</v>
+      </c>
+      <c r="F5">
+        <v>95</v>
+      </c>
+      <c r="G5">
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -3077,7 +2816,7 @@
         <v>0</v>
       </c>
       <c r="B6">
-        <v>1269915</v>
+        <v>3760185</v>
       </c>
       <c r="C6">
         <v>1282475</v>
@@ -3087,179 +2826,174 @@
       </c>
       <c r="E6">
         <v>1263833</v>
+      </c>
+      <c r="F6">
+        <v>1039483</v>
+      </c>
+      <c r="G6">
+        <v>13389</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7">
+        <f>B3/2932</f>
+        <v>10.37619372442019</v>
+      </c>
+      <c r="C7">
+        <f>C3/2932</f>
+        <v>9.2919508867667115</v>
+      </c>
+      <c r="D7">
+        <f t="shared" ref="D7:G7" si="0">D3/2932</f>
+        <v>9.3086630286493861</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>9.3935879945429743</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>10.898021828103683</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>9.254433833560709</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8">
+        <f t="shared" ref="B8:C10" si="1">B4/2932</f>
+        <v>12.251364256480219</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="1"/>
+        <v>8.4229195088676665</v>
+      </c>
+      <c r="D8">
+        <f t="shared" ref="D8:G8" si="2">D4/2932</f>
+        <v>8.1459754433833567</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="2"/>
+        <v>7.8782401091405188</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="2"/>
+        <v>8.5354706684856758</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="2"/>
+        <v>8.2186221009549794</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" t="s">
-        <v>4</v>
-      </c>
-      <c r="F9" t="s">
-        <v>5</v>
-      </c>
-      <c r="G9" t="s">
-        <v>6</v>
+        <v>23</v>
+      </c>
+      <c r="B9">
+        <f>B5/2932*1000</f>
+        <v>42.291950886766713</v>
+      </c>
+      <c r="C9">
+        <f>C5/2932*1000</f>
+        <v>39.563437926330153</v>
+      </c>
+      <c r="D9">
+        <f t="shared" ref="D9:G9" si="3">D5/2932*1000</f>
+        <v>39.563437926330153</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="3"/>
+        <v>39.563437926330153</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="3"/>
+        <v>32.401091405184175</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="3"/>
+        <v>17.053206002728512</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11">
-        <v>31041</v>
-      </c>
-      <c r="C11">
-        <v>30502</v>
-      </c>
-      <c r="D11">
-        <v>30465</v>
-      </c>
-      <c r="E11">
-        <v>30553</v>
-      </c>
-      <c r="F11">
-        <v>33527</v>
-      </c>
-      <c r="G11">
-        <v>33448</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12">
-        <v>27985</v>
-      </c>
-      <c r="C12">
-        <v>27807</v>
-      </c>
-      <c r="D12">
-        <v>27400</v>
-      </c>
-      <c r="E12">
-        <v>27087</v>
-      </c>
-      <c r="F12">
-        <v>27894</v>
-      </c>
-      <c r="G12">
-        <v>26851</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13">
-        <v>99</v>
-      </c>
-      <c r="C13">
-        <v>95</v>
-      </c>
-      <c r="D13">
-        <v>95</v>
-      </c>
-      <c r="E13">
-        <v>96</v>
-      </c>
-      <c r="F13">
-        <v>89</v>
-      </c>
-      <c r="G13">
-        <v>77</v>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="1"/>
+        <v>1282.4641882673943</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="1"/>
+        <v>437.40620736698497</v>
+      </c>
+      <c r="D10">
+        <f t="shared" ref="D10:G10" si="4">D6/2932</f>
+        <v>437.40620736698497</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="4"/>
+        <v>431.04809004092772</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="4"/>
+        <v>354.53035470668488</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="4"/>
+        <v>4.5665075034106408</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>0</v>
-      </c>
-      <c r="B14">
-        <v>156670</v>
-      </c>
-      <c r="C14">
-        <v>154874</v>
-      </c>
-      <c r="D14">
-        <v>154874</v>
-      </c>
-      <c r="E14">
-        <v>155056</v>
-      </c>
-      <c r="F14">
-        <v>73949</v>
-      </c>
-      <c r="G14">
-        <v>17868</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B15">
-        <f>(B11/158/20)</f>
-        <v>9.8231012658227854</v>
-      </c>
-      <c r="C15">
-        <f t="shared" ref="C15:G16" si="0">(C11/158/20)</f>
-        <v>9.6525316455696206</v>
-      </c>
-      <c r="D15">
-        <f t="shared" si="0"/>
-        <v>9.6408227848101262</v>
-      </c>
-      <c r="E15">
-        <f t="shared" si="0"/>
-        <v>9.6686708860759492</v>
-      </c>
-      <c r="F15">
-        <f t="shared" si="0"/>
-        <v>10.609810126582278</v>
-      </c>
-      <c r="G15">
-        <f t="shared" si="0"/>
-        <v>10.58481012658228</v>
+        <v>7</v>
+      </c>
+      <c r="B14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" t="s">
+        <v>3</v>
+      </c>
+      <c r="F14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G14" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="B16">
-        <f t="shared" ref="B16:G16" si="1">(B12/158/20)</f>
-        <v>8.8560126582278489</v>
+        <v>30633</v>
       </c>
       <c r="C16">
-        <f t="shared" si="1"/>
-        <v>8.7996835443037984</v>
+        <v>30502</v>
       </c>
       <c r="D16">
-        <f t="shared" si="1"/>
-        <v>8.6708860759493671</v>
+        <v>30465</v>
       </c>
       <c r="E16">
-        <f t="shared" si="1"/>
-        <v>8.5718354430379744</v>
+        <v>30553</v>
       </c>
       <c r="F16">
-        <f t="shared" si="1"/>
-        <v>8.8272151898734172</v>
+        <v>33527</v>
       </c>
       <c r="G16">
-        <f t="shared" si="1"/>
-        <v>8.4971518987341774</v>
+        <v>33448</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
@@ -3267,230 +3001,230 @@
         <v>26</v>
       </c>
       <c r="B17">
-        <f>(B13/158/20)*1000</f>
-        <v>31.329113924050635</v>
+        <v>38071</v>
       </c>
       <c r="C17">
-        <f t="shared" ref="C17:G17" si="2">(C13/158/20)*1000</f>
-        <v>30.063291139240508</v>
+        <v>27807</v>
       </c>
       <c r="D17">
-        <f t="shared" si="2"/>
-        <v>30.063291139240508</v>
+        <v>27400</v>
       </c>
       <c r="E17">
-        <f t="shared" si="2"/>
-        <v>30.37974683544304</v>
+        <v>27894</v>
       </c>
       <c r="F17">
-        <f t="shared" si="2"/>
-        <v>28.164556962025319</v>
+        <v>27087</v>
       </c>
       <c r="G17">
-        <f t="shared" si="2"/>
-        <v>24.367088607594933</v>
+        <v>26851</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="B18">
-        <f t="shared" ref="B18:G18" si="3">(B14/158/20)</f>
-        <v>49.579113924050631</v>
+        <v>125</v>
       </c>
       <c r="C18">
-        <f t="shared" si="3"/>
-        <v>49.010759493670882</v>
+        <v>95</v>
       </c>
       <c r="D18">
-        <f t="shared" si="3"/>
-        <v>49.010759493670882</v>
+        <v>95</v>
       </c>
       <c r="E18">
-        <f t="shared" si="3"/>
-        <v>49.068354430379749</v>
+        <v>96</v>
       </c>
       <c r="F18">
-        <f t="shared" si="3"/>
-        <v>23.401582278481012</v>
+        <v>89</v>
       </c>
       <c r="G18">
-        <f t="shared" si="3"/>
-        <v>5.6544303797468354</v>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19">
+        <v>4335578</v>
+      </c>
+      <c r="C19">
+        <v>154874</v>
+      </c>
+      <c r="D19">
+        <v>154874</v>
+      </c>
+      <c r="E19">
+        <v>155056</v>
+      </c>
+      <c r="F19">
+        <v>73949</v>
+      </c>
+      <c r="G19">
+        <v>17868</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20">
+        <f>(B16/158/20)</f>
+        <v>9.6939873417721518</v>
+      </c>
+      <c r="C20">
+        <f t="shared" ref="C20:G20" si="5">(C16/158/20)</f>
+        <v>9.6525316455696206</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="5"/>
+        <v>9.6408227848101262</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="5"/>
+        <v>9.6686708860759492</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="5"/>
+        <v>10.609810126582278</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="5"/>
+        <v>10.58481012658228</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>22</v>
-      </c>
-      <c r="B21" t="s">
-        <v>2</v>
-      </c>
-      <c r="C21" t="s">
-        <v>3</v>
-      </c>
-      <c r="D21" t="s">
-        <v>7</v>
-      </c>
-      <c r="E21" t="s">
-        <v>4</v>
-      </c>
-      <c r="F21" t="s">
-        <v>5</v>
-      </c>
-      <c r="G21" t="s">
-        <v>6</v>
+        <v>25</v>
+      </c>
+      <c r="B21">
+        <f t="shared" ref="B21:G21" si="6">(B17/158/20)</f>
+        <v>12.047784810126583</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="6"/>
+        <v>8.7996835443037984</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="6"/>
+        <v>8.6708860759493671</v>
+      </c>
+      <c r="E21">
+        <f>(E17/158/20)</f>
+        <v>8.8272151898734172</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="6"/>
+        <v>8.5718354430379744</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="6"/>
+        <v>8.4971518987341774</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22">
+        <f>(B18/158/20)*1000</f>
+        <v>39.556962025316459</v>
+      </c>
+      <c r="C22">
+        <f t="shared" ref="C22:G22" si="7">(C18/158/20)*1000</f>
+        <v>30.063291139240508</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="7"/>
+        <v>30.063291139240508</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="7"/>
+        <v>30.37974683544304</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="7"/>
+        <v>28.164556962025319</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="7"/>
+        <v>24.367088607594933</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="B23">
-        <v>1721</v>
+        <f t="shared" ref="B23:G23" si="8">(B19/158/20)</f>
+        <v>1372.0183544303798</v>
       </c>
       <c r="C23">
-        <v>1708</v>
+        <f t="shared" si="8"/>
+        <v>49.010759493670882</v>
       </c>
       <c r="D23">
-        <v>1710</v>
+        <f t="shared" si="8"/>
+        <v>49.010759493670882</v>
       </c>
       <c r="E23">
-        <v>1847</v>
+        <f t="shared" si="8"/>
+        <v>49.068354430379749</v>
       </c>
       <c r="F23">
-        <v>2083</v>
+        <f t="shared" si="8"/>
+        <v>23.401582278481012</v>
       </c>
       <c r="G23">
-        <v>1951</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>10</v>
-      </c>
-      <c r="B24">
-        <v>1753</v>
-      </c>
-      <c r="C24">
-        <v>1744</v>
-      </c>
-      <c r="D24">
-        <v>1679</v>
-      </c>
-      <c r="E24">
-        <v>1828</v>
-      </c>
-      <c r="F24">
-        <v>1729</v>
-      </c>
-      <c r="G24">
-        <v>1642</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>11</v>
-      </c>
-      <c r="B25">
-        <v>6</v>
-      </c>
-      <c r="C25">
-        <v>6</v>
-      </c>
-      <c r="D25">
-        <v>6</v>
-      </c>
-      <c r="E25">
-        <v>5</v>
-      </c>
-      <c r="F25">
-        <v>5</v>
-      </c>
-      <c r="G25">
-        <v>4</v>
+        <f t="shared" si="8"/>
+        <v>5.6544303797468354</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>0</v>
-      </c>
-      <c r="B26">
-        <v>81394</v>
-      </c>
-      <c r="C26">
-        <v>85013</v>
-      </c>
-      <c r="D26">
-        <v>85013</v>
-      </c>
-      <c r="E26">
-        <v>108203</v>
-      </c>
-      <c r="F26">
-        <v>30584</v>
-      </c>
-      <c r="G26">
-        <v>2181</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>23</v>
-      </c>
-      <c r="B27">
-        <f>(B23/7/27)</f>
-        <v>9.105820105820106</v>
-      </c>
-      <c r="C27">
-        <f t="shared" ref="C27:G27" si="4">(C23/7/27)</f>
-        <v>9.0370370370370363</v>
-      </c>
-      <c r="D27">
-        <f t="shared" si="4"/>
-        <v>9.0476190476190474</v>
-      </c>
-      <c r="E27">
-        <f t="shared" si="4"/>
-        <v>9.7724867724867721</v>
-      </c>
-      <c r="F27">
-        <f t="shared" si="4"/>
-        <v>11.02116402116402</v>
-      </c>
-      <c r="G27">
-        <f t="shared" si="4"/>
-        <v>10.322751322751323</v>
+        <v>20</v>
+      </c>
+      <c r="B26" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" t="s">
+        <v>2</v>
+      </c>
+      <c r="D26" t="s">
+        <v>6</v>
+      </c>
+      <c r="E26" t="s">
+        <v>3</v>
+      </c>
+      <c r="F26" t="s">
+        <v>4</v>
+      </c>
+      <c r="G26" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="B28">
-        <f t="shared" ref="B28:G28" si="5">(B24/7/27)</f>
-        <v>9.2751322751322753</v>
+        <v>1844</v>
       </c>
       <c r="C28">
-        <f t="shared" si="5"/>
-        <v>9.2275132275132279</v>
+        <v>1708</v>
       </c>
       <c r="D28">
-        <f t="shared" si="5"/>
-        <v>8.8835978835978846</v>
+        <v>1710</v>
       </c>
       <c r="E28">
-        <f t="shared" si="5"/>
-        <v>9.6719576719576725</v>
+        <v>1847</v>
       </c>
       <c r="F28">
-        <f t="shared" si="5"/>
-        <v>9.1481481481481488</v>
+        <v>2083</v>
       </c>
       <c r="G28">
-        <f t="shared" si="5"/>
-        <v>8.6878306878306883</v>
+        <v>1951</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
@@ -3498,257 +3232,384 @@
         <v>26</v>
       </c>
       <c r="B29">
-        <f>(B25/7/27)*1000</f>
-        <v>31.746031746031743</v>
+        <v>2295</v>
       </c>
       <c r="C29">
-        <f t="shared" ref="C29:G29" si="6">(C25/7/27)*1000</f>
-        <v>31.746031746031743</v>
+        <v>1744</v>
       </c>
       <c r="D29">
-        <f t="shared" si="6"/>
-        <v>31.746031746031743</v>
+        <v>1679</v>
       </c>
       <c r="E29">
-        <f t="shared" si="6"/>
-        <v>26.455026455026456</v>
+        <v>1828</v>
       </c>
       <c r="F29">
-        <f t="shared" si="6"/>
-        <v>26.455026455026456</v>
+        <v>1729</v>
       </c>
       <c r="G29">
-        <f t="shared" si="6"/>
-        <v>21.164021164021165</v>
+        <v>1642</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="B30">
-        <f t="shared" ref="B30:G30" si="7">(B26/7/27)</f>
-        <v>430.65608465608466</v>
+        <v>7</v>
       </c>
       <c r="C30">
-        <f t="shared" si="7"/>
-        <v>449.80423280423281</v>
+        <v>6</v>
       </c>
       <c r="D30">
-        <f t="shared" si="7"/>
-        <v>449.80423280423281</v>
+        <v>6</v>
       </c>
       <c r="E30">
-        <f t="shared" si="7"/>
-        <v>572.50264550264558</v>
+        <v>5</v>
       </c>
       <c r="F30">
-        <f t="shared" si="7"/>
-        <v>161.82010582010582</v>
+        <v>5</v>
       </c>
       <c r="G30">
-        <f t="shared" si="7"/>
-        <v>11.53968253968254</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31">
+        <v>245791</v>
+      </c>
+      <c r="C31">
+        <v>85013</v>
+      </c>
+      <c r="D31">
+        <v>85013</v>
+      </c>
+      <c r="E31">
+        <v>108203</v>
+      </c>
+      <c r="F31">
+        <v>30584</v>
+      </c>
+      <c r="G31">
+        <v>2181</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>21</v>
+      </c>
+      <c r="B32">
+        <f>(B28/7/27)</f>
+        <v>9.7566137566137581</v>
+      </c>
+      <c r="C32">
+        <f t="shared" ref="C32:G32" si="9">(C28/7/27)</f>
+        <v>9.0370370370370363</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="9"/>
+        <v>9.0476190476190474</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="9"/>
+        <v>9.7724867724867721</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="9"/>
+        <v>11.02116402116402</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="9"/>
+        <v>10.322751322751323</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>1</v>
-      </c>
-      <c r="B33" t="s">
-        <v>12</v>
-      </c>
-      <c r="C33" t="s">
-        <v>13</v>
-      </c>
-      <c r="D33" t="s">
-        <v>14</v>
-      </c>
-      <c r="E33" t="s">
-        <v>15</v>
-      </c>
-      <c r="F33" t="s">
-        <v>16</v>
-      </c>
-      <c r="G33" t="s">
-        <v>17</v>
-      </c>
-      <c r="H33" t="s">
-        <v>18</v>
-      </c>
-      <c r="I33" t="s">
-        <v>19</v>
-      </c>
-      <c r="J33" t="s">
-        <v>20</v>
+        <v>25</v>
+      </c>
+      <c r="B33">
+        <f t="shared" ref="B33:G33" si="10">(B29/7/27)</f>
+        <v>12.142857142857142</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="10"/>
+        <v>9.2275132275132279</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="10"/>
+        <v>8.8835978835978846</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="10"/>
+        <v>9.6719576719576725</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="10"/>
+        <v>9.1481481481481488</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="10"/>
+        <v>8.6878306878306883</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="B34">
-        <v>27244</v>
+        <f>(B30/7/27)*1000</f>
+        <v>37.037037037037038</v>
       </c>
       <c r="C34">
-        <v>27144</v>
-      </c>
-      <c r="D34" s="2">
-        <v>27144</v>
-      </c>
-      <c r="E34" s="2">
-        <v>27156</v>
+        <f t="shared" ref="C34:G34" si="11">(C30/7/27)*1000</f>
+        <v>31.746031746031743</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="11"/>
+        <v>31.746031746031743</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="11"/>
+        <v>26.455026455026456</v>
       </c>
       <c r="F34">
-        <v>27160</v>
+        <f t="shared" si="11"/>
+        <v>26.455026455026456</v>
       </c>
       <c r="G34">
-        <v>27160</v>
-      </c>
-      <c r="H34">
-        <v>27177</v>
-      </c>
-      <c r="I34" s="1">
-        <v>27096</v>
-      </c>
-      <c r="J34">
-        <v>27160</v>
+        <f t="shared" si="11"/>
+        <v>21.164021164021165</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="B35">
-        <v>24696</v>
+        <f t="shared" ref="B35:G35" si="12">(B31/7/27)</f>
+        <v>1300.4814814814815</v>
       </c>
       <c r="C35">
-        <v>24680</v>
-      </c>
-      <c r="D35" s="2">
-        <v>24680</v>
-      </c>
-      <c r="E35" s="2">
-        <v>24717</v>
+        <f t="shared" si="12"/>
+        <v>449.80423280423281</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="12"/>
+        <v>449.80423280423281</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="12"/>
+        <v>572.50264550264558</v>
       </c>
       <c r="F35">
-        <v>24722</v>
+        <f t="shared" si="12"/>
+        <v>161.82010582010582</v>
       </c>
       <c r="G35">
-        <v>24722</v>
-      </c>
-      <c r="H35">
-        <v>24719</v>
-      </c>
-      <c r="I35" s="1">
-        <v>24653</v>
-      </c>
-      <c r="J35">
-        <v>24722</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>11</v>
-      </c>
-      <c r="B36">
-        <v>116</v>
-      </c>
-      <c r="C36">
-        <v>116</v>
-      </c>
-      <c r="D36" s="2">
-        <v>116</v>
-      </c>
-      <c r="E36" s="2">
-        <v>116</v>
-      </c>
-      <c r="F36">
-        <v>116</v>
-      </c>
-      <c r="G36">
-        <v>116</v>
-      </c>
-      <c r="H36">
-        <v>116</v>
-      </c>
-      <c r="I36">
-        <v>116</v>
-      </c>
-      <c r="J36">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>0</v>
-      </c>
-      <c r="B37">
-        <v>1282475</v>
-      </c>
-      <c r="C37">
-        <v>1270051</v>
-      </c>
-      <c r="D37" s="2">
-        <v>1270051</v>
-      </c>
-      <c r="E37" s="2">
-        <v>1264990</v>
-      </c>
-      <c r="F37" s="1">
-        <v>1264854</v>
-      </c>
-      <c r="G37" s="1">
-        <v>1264854</v>
-      </c>
-      <c r="H37">
-        <v>1265558</v>
-      </c>
-      <c r="I37">
-        <v>1284166</v>
-      </c>
-      <c r="J37" s="1">
-        <v>1264854</v>
+        <f t="shared" si="12"/>
+        <v>11.53968253968254</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>21</v>
-      </c>
-      <c r="B38">
-        <f>B34+B35+B36+(B37/100)</f>
+        <v>1</v>
+      </c>
+      <c r="B38" t="s">
+        <v>10</v>
+      </c>
+      <c r="C38" t="s">
+        <v>11</v>
+      </c>
+      <c r="D38" t="s">
+        <v>12</v>
+      </c>
+      <c r="E38" t="s">
+        <v>13</v>
+      </c>
+      <c r="F38" t="s">
+        <v>14</v>
+      </c>
+      <c r="G38" t="s">
+        <v>15</v>
+      </c>
+      <c r="H38" t="s">
+        <v>16</v>
+      </c>
+      <c r="I38" t="s">
+        <v>17</v>
+      </c>
+      <c r="J38" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B39">
+        <v>27244</v>
+      </c>
+      <c r="C39">
+        <v>27144</v>
+      </c>
+      <c r="D39" s="2">
+        <v>27144</v>
+      </c>
+      <c r="E39" s="2">
+        <v>27156</v>
+      </c>
+      <c r="F39">
+        <v>27160</v>
+      </c>
+      <c r="G39">
+        <v>27160</v>
+      </c>
+      <c r="H39">
+        <v>27177</v>
+      </c>
+      <c r="I39" s="1">
+        <v>27096</v>
+      </c>
+      <c r="J39">
+        <v>27160</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>26</v>
+      </c>
+      <c r="B40">
+        <v>24696</v>
+      </c>
+      <c r="C40">
+        <v>24680</v>
+      </c>
+      <c r="D40" s="2">
+        <v>24680</v>
+      </c>
+      <c r="E40" s="2">
+        <v>24717</v>
+      </c>
+      <c r="F40">
+        <v>24722</v>
+      </c>
+      <c r="G40">
+        <v>24722</v>
+      </c>
+      <c r="H40">
+        <v>24719</v>
+      </c>
+      <c r="I40" s="1">
+        <v>24653</v>
+      </c>
+      <c r="J40">
+        <v>24722</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>9</v>
+      </c>
+      <c r="B41">
+        <v>116</v>
+      </c>
+      <c r="C41">
+        <v>116</v>
+      </c>
+      <c r="D41" s="2">
+        <v>116</v>
+      </c>
+      <c r="E41" s="2">
+        <v>116</v>
+      </c>
+      <c r="F41">
+        <v>116</v>
+      </c>
+      <c r="G41">
+        <v>116</v>
+      </c>
+      <c r="H41">
+        <v>116</v>
+      </c>
+      <c r="I41">
+        <v>116</v>
+      </c>
+      <c r="J41">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>0</v>
+      </c>
+      <c r="B42">
+        <v>1282475</v>
+      </c>
+      <c r="C42">
+        <v>1270051</v>
+      </c>
+      <c r="D42" s="2">
+        <v>1270051</v>
+      </c>
+      <c r="E42" s="2">
+        <v>1264990</v>
+      </c>
+      <c r="F42" s="1">
+        <v>1264854</v>
+      </c>
+      <c r="G42" s="1">
+        <v>1264854</v>
+      </c>
+      <c r="H42">
+        <v>1265558</v>
+      </c>
+      <c r="I42">
+        <v>1284166</v>
+      </c>
+      <c r="J42" s="1">
+        <v>1264854</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>19</v>
+      </c>
+      <c r="B43">
+        <f>B39+B40+B41+(B42/100)</f>
         <v>64880.75</v>
       </c>
-      <c r="C38">
-        <f t="shared" ref="C38:J38" si="8">C34+C35+C36+(C37/100)</f>
+      <c r="C43">
+        <f t="shared" ref="C43:J43" si="13">C39+C40+C41+(C42/100)</f>
         <v>64640.51</v>
       </c>
-      <c r="D38">
-        <f t="shared" si="8"/>
+      <c r="D43">
+        <f t="shared" si="13"/>
         <v>64640.51</v>
       </c>
-      <c r="E38">
-        <f t="shared" si="8"/>
+      <c r="E43">
+        <f t="shared" si="13"/>
         <v>64638.9</v>
       </c>
-      <c r="F38">
-        <f t="shared" si="8"/>
+      <c r="F43">
+        <f t="shared" si="13"/>
         <v>64646.54</v>
       </c>
-      <c r="G38">
-        <f t="shared" si="8"/>
+      <c r="G43">
+        <f t="shared" si="13"/>
         <v>64646.54</v>
       </c>
-      <c r="H38">
-        <f t="shared" si="8"/>
+      <c r="H43">
+        <f t="shared" si="13"/>
         <v>64667.58</v>
       </c>
-      <c r="I38">
-        <f t="shared" si="8"/>
+      <c r="I43">
+        <f t="shared" si="13"/>
         <v>64706.66</v>
       </c>
-      <c r="J38">
-        <f t="shared" si="8"/>
+      <c r="J43">
+        <f t="shared" si="13"/>
         <v>64646.54</v>
       </c>
     </row>

</xml_diff>